<commit_message>
Updated text for new tables
</commit_message>
<xml_diff>
--- a/data/maingraphs-code-size-table3a.xlsx
+++ b/data/maingraphs-code-size-table3a.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="28125"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="-20" windowWidth="33600" windowHeight="20540" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16060" tabRatio="500" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="main table" sheetId="1" r:id="rId1"/>
@@ -1542,7 +1542,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:R66"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A18" workbookViewId="0">
+    <sheetView topLeftCell="A18" workbookViewId="0">
       <selection activeCell="B36" sqref="B36:O63"/>
     </sheetView>
   </sheetViews>
@@ -2846,59 +2846,59 @@
         <v>14</v>
       </c>
       <c r="B36" s="4">
-        <f>B4</f>
+        <f t="shared" ref="B36:O36" si="0">B4</f>
         <v>449.2</v>
       </c>
       <c r="C36" s="4">
-        <f>C4</f>
+        <f t="shared" si="0"/>
         <v>298</v>
       </c>
       <c r="D36" s="4">
-        <f>D4</f>
+        <f t="shared" si="0"/>
         <v>208.2</v>
       </c>
       <c r="E36" s="4">
-        <f>E4</f>
+        <f t="shared" si="0"/>
         <v>287.2</v>
       </c>
       <c r="F36" s="4">
-        <f>F4</f>
+        <f t="shared" si="0"/>
         <v>166</v>
       </c>
       <c r="G36" s="4">
-        <f>G4</f>
+        <f t="shared" si="0"/>
         <v>239.3</v>
       </c>
       <c r="H36" s="4">
-        <f>H4</f>
+        <f t="shared" si="0"/>
         <v>94.9</v>
       </c>
       <c r="I36" s="4">
-        <f>I4</f>
+        <f t="shared" si="0"/>
         <v>316.3</v>
       </c>
       <c r="J36" s="4">
-        <f>J4</f>
+        <f t="shared" si="0"/>
         <v>186.4</v>
       </c>
       <c r="K36" s="4">
-        <f>K4</f>
+        <f t="shared" si="0"/>
         <v>159.4</v>
       </c>
       <c r="L36" s="4">
-        <f>L4</f>
+        <f t="shared" si="0"/>
         <v>255</v>
       </c>
       <c r="M36" s="4">
-        <f>M4</f>
+        <f t="shared" si="0"/>
         <v>26.2</v>
       </c>
       <c r="N36" s="4">
-        <f>N4</f>
+        <f t="shared" si="0"/>
         <v>238.5</v>
       </c>
       <c r="O36" s="4">
-        <f>O4</f>
+        <f t="shared" si="0"/>
         <v>225</v>
       </c>
     </row>
@@ -2907,59 +2907,59 @@
         <v>15</v>
       </c>
       <c r="B37" s="4">
-        <f>B5</f>
+        <f t="shared" ref="B37:O37" si="1">B5</f>
         <v>159.30000000000001</v>
       </c>
       <c r="C37" s="4">
-        <f>C5</f>
+        <f t="shared" si="1"/>
         <v>99.3</v>
       </c>
       <c r="D37" s="4">
-        <f>D5</f>
+        <f t="shared" si="1"/>
         <v>71.2</v>
       </c>
       <c r="E37" s="4">
-        <f>E5</f>
+        <f t="shared" si="1"/>
         <v>140.6</v>
       </c>
       <c r="F37" s="4">
-        <f>F5</f>
+        <f t="shared" si="1"/>
         <v>110.7</v>
       </c>
       <c r="G37" s="4">
-        <f>G5</f>
+        <f t="shared" si="1"/>
         <v>108.6</v>
       </c>
       <c r="H37" s="4">
-        <f>H5</f>
+        <f t="shared" si="1"/>
         <v>47.7</v>
       </c>
       <c r="I37" s="4">
-        <f>I5</f>
+        <f t="shared" si="1"/>
         <v>92.6</v>
       </c>
       <c r="J37" s="4">
-        <f>J5</f>
+        <f t="shared" si="1"/>
         <v>60.7</v>
       </c>
       <c r="K37" s="4">
-        <f>K5</f>
+        <f t="shared" si="1"/>
         <v>69.599999999999994</v>
       </c>
       <c r="L37" s="4">
-        <f>L5</f>
+        <f t="shared" si="1"/>
         <v>78.099999999999994</v>
       </c>
       <c r="M37" s="4">
-        <f>M5</f>
+        <f t="shared" si="1"/>
         <v>31.7</v>
       </c>
       <c r="N37" s="4">
-        <f>N5</f>
+        <f t="shared" si="1"/>
         <v>93.9</v>
       </c>
       <c r="O37" s="4">
-        <f>O5</f>
+        <f t="shared" si="1"/>
         <v>89.5</v>
       </c>
     </row>
@@ -2968,59 +2968,59 @@
         <v>16</v>
       </c>
       <c r="B38" s="4">
-        <f>B6</f>
+        <f t="shared" ref="B38:O38" si="2">B6</f>
         <v>128.80000000000001</v>
       </c>
       <c r="C38" s="4">
-        <f>C6</f>
+        <f t="shared" si="2"/>
         <v>65.8</v>
       </c>
       <c r="D38" s="4">
-        <f>D6</f>
+        <f t="shared" si="2"/>
         <v>76.7</v>
       </c>
       <c r="E38" s="4">
-        <f>E6</f>
+        <f t="shared" si="2"/>
         <v>68.900000000000006</v>
       </c>
       <c r="F38" s="4">
-        <f>F6</f>
+        <f t="shared" si="2"/>
         <v>40.799999999999997</v>
       </c>
       <c r="G38" s="4">
-        <f>G6</f>
+        <f t="shared" si="2"/>
         <v>56.5</v>
       </c>
       <c r="H38" s="4">
-        <f>H6</f>
+        <f t="shared" si="2"/>
         <v>20.3</v>
       </c>
       <c r="I38" s="4">
-        <f>I6</f>
+        <f t="shared" si="2"/>
         <v>103.2</v>
       </c>
       <c r="J38" s="4">
-        <f>J6</f>
+        <f t="shared" si="2"/>
         <v>71.400000000000006</v>
       </c>
       <c r="K38" s="4">
-        <f>K6</f>
+        <f t="shared" si="2"/>
         <v>51.6</v>
       </c>
       <c r="L38" s="4">
-        <f>L6</f>
+        <f t="shared" si="2"/>
         <v>75.900000000000006</v>
       </c>
       <c r="M38" s="4">
-        <f>M6</f>
+        <f t="shared" si="2"/>
         <v>22.6</v>
       </c>
       <c r="N38" s="4">
-        <f>N6</f>
+        <f t="shared" si="2"/>
         <v>56.4</v>
       </c>
       <c r="O38" s="4">
-        <f>O6</f>
+        <f t="shared" si="2"/>
         <v>64.5</v>
       </c>
     </row>
@@ -3029,59 +3029,59 @@
         <v>17</v>
       </c>
       <c r="B39" s="4">
-        <f>B7</f>
+        <f t="shared" ref="B39:O39" si="3">B7</f>
         <v>1.7</v>
       </c>
       <c r="C39" s="4">
-        <f>C7</f>
+        <f t="shared" si="3"/>
         <v>17.399999999999999</v>
       </c>
       <c r="D39" s="4">
-        <f>D7</f>
+        <f t="shared" si="3"/>
         <v>9.6</v>
       </c>
       <c r="E39" s="4">
-        <f>E7</f>
+        <f t="shared" si="3"/>
         <v>10.1</v>
       </c>
       <c r="F39" s="4">
-        <f>F7</f>
+        <f t="shared" si="3"/>
         <v>-3.6</v>
       </c>
       <c r="G39" s="4">
-        <f>G7</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="H39" s="4">
-        <f>H7</f>
+        <f t="shared" si="3"/>
         <v>2.5</v>
       </c>
       <c r="I39" s="4">
-        <f>I7</f>
+        <f t="shared" si="3"/>
         <v>14.7</v>
       </c>
       <c r="J39" s="4">
-        <f>J7</f>
+        <f t="shared" si="3"/>
         <v>5.7</v>
       </c>
       <c r="K39" s="4">
-        <f>K7</f>
+        <f t="shared" si="3"/>
         <v>-3.1</v>
       </c>
       <c r="L39" s="4">
-        <f>L7</f>
+        <f t="shared" si="3"/>
         <v>24.1</v>
       </c>
       <c r="M39" s="4">
-        <f>M7</f>
+        <f t="shared" si="3"/>
         <v>-14.3</v>
       </c>
       <c r="N39" s="4">
-        <f>N7</f>
+        <f t="shared" si="3"/>
         <v>15.1</v>
       </c>
       <c r="O39" s="4">
-        <f>O7</f>
+        <f t="shared" si="3"/>
         <v>6.1</v>
       </c>
     </row>
@@ -3090,59 +3090,59 @@
         <v>19</v>
       </c>
       <c r="B40" s="4">
-        <f>B8</f>
+        <f t="shared" ref="B40:O40" si="4">B8</f>
         <v>159.30000000000001</v>
       </c>
       <c r="C40" s="4">
-        <f>C8</f>
+        <f t="shared" si="4"/>
         <v>115.4</v>
       </c>
       <c r="D40" s="4">
-        <f>D8</f>
+        <f t="shared" si="4"/>
         <v>50.7</v>
       </c>
       <c r="E40" s="4">
-        <f>E8</f>
+        <f t="shared" si="4"/>
         <v>67.599999999999994</v>
       </c>
       <c r="F40" s="4">
-        <f>F8</f>
+        <f t="shared" si="4"/>
         <v>18</v>
       </c>
       <c r="G40" s="4">
-        <f>G8</f>
+        <f t="shared" si="4"/>
         <v>74.3</v>
       </c>
       <c r="H40" s="4">
-        <f>H8</f>
+        <f t="shared" si="4"/>
         <v>24.5</v>
       </c>
       <c r="I40" s="4">
-        <f>I8</f>
+        <f t="shared" si="4"/>
         <v>105.8</v>
       </c>
       <c r="J40" s="4">
-        <f>J8</f>
+        <f t="shared" si="4"/>
         <v>48.6</v>
       </c>
       <c r="K40" s="4">
-        <f>K8</f>
+        <f t="shared" si="4"/>
         <v>41.2</v>
       </c>
       <c r="L40" s="4">
-        <f>L8</f>
+        <f t="shared" si="4"/>
         <v>76.900000000000006</v>
       </c>
       <c r="M40" s="4">
-        <f>M8</f>
+        <f t="shared" si="4"/>
         <v>-13.8</v>
       </c>
       <c r="N40" s="4">
-        <f>N8</f>
+        <f t="shared" si="4"/>
         <v>73.099999999999994</v>
       </c>
       <c r="O40" s="4">
-        <f>O8</f>
+        <f t="shared" si="4"/>
         <v>64.7</v>
       </c>
     </row>
@@ -3174,55 +3174,55 @@
         <v>-195</v>
       </c>
       <c r="C42" s="4">
-        <f t="shared" ref="C42:O42" si="0">C17-C16</f>
+        <f t="shared" ref="C42:O42" si="5">C17-C16</f>
         <v>-58.400000000000006</v>
       </c>
       <c r="D42" s="4">
-        <f t="shared" si="0"/>
+        <f t="shared" si="5"/>
         <v>-26</v>
       </c>
       <c r="E42" s="4">
-        <f t="shared" si="0"/>
+        <f t="shared" si="5"/>
         <v>-124.19999999999999</v>
       </c>
       <c r="F42" s="4">
-        <f t="shared" si="0"/>
+        <f t="shared" si="5"/>
         <v>45.900000000000006</v>
       </c>
       <c r="G42" s="4">
-        <f t="shared" si="0"/>
+        <f t="shared" si="5"/>
         <v>110.19999999999999</v>
       </c>
       <c r="H42" s="4">
-        <f t="shared" si="0"/>
+        <f t="shared" si="5"/>
         <v>4.5</v>
       </c>
       <c r="I42" s="4">
-        <f t="shared" si="0"/>
+        <f t="shared" si="5"/>
         <v>-47.400000000000034</v>
       </c>
       <c r="J42" s="4">
-        <f t="shared" si="0"/>
+        <f t="shared" si="5"/>
         <v>4.2999999999999829</v>
       </c>
       <c r="K42" s="4">
-        <f t="shared" si="0"/>
+        <f t="shared" si="5"/>
         <v>-31.200000000000017</v>
       </c>
       <c r="L42" s="4">
-        <f t="shared" si="0"/>
+        <f t="shared" si="5"/>
         <v>-27.699999999999989</v>
       </c>
       <c r="M42" s="4">
-        <f t="shared" si="0"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="N42" s="4">
-        <f t="shared" si="0"/>
+        <f t="shared" si="5"/>
         <v>-12.699999999999989</v>
       </c>
       <c r="O42" s="4">
-        <f t="shared" si="0"/>
+        <f t="shared" si="5"/>
         <v>-27.5</v>
       </c>
     </row>
@@ -3251,307 +3251,307 @@
         <v>total</v>
       </c>
       <c r="B44" s="4">
-        <f t="shared" ref="B44:O44" si="1">B10</f>
+        <f t="shared" ref="B44:O44" si="6">B10</f>
         <v>254.2</v>
       </c>
       <c r="C44" s="4">
-        <f t="shared" si="1"/>
+        <f t="shared" si="6"/>
         <v>239.6</v>
       </c>
       <c r="D44" s="4">
-        <f t="shared" si="1"/>
+        <f t="shared" si="6"/>
         <v>182.2</v>
       </c>
       <c r="E44" s="4">
-        <f t="shared" si="1"/>
+        <f t="shared" si="6"/>
         <v>163</v>
       </c>
       <c r="F44" s="4">
-        <f t="shared" si="1"/>
+        <f t="shared" si="6"/>
         <v>211.9</v>
       </c>
       <c r="G44" s="4">
-        <f t="shared" si="1"/>
+        <f t="shared" si="6"/>
         <v>349.5</v>
       </c>
       <c r="H44" s="4">
-        <f t="shared" si="1"/>
+        <f t="shared" si="6"/>
         <v>99.4</v>
       </c>
       <c r="I44" s="4">
-        <f t="shared" si="1"/>
+        <f t="shared" si="6"/>
         <v>268.89999999999998</v>
       </c>
       <c r="J44" s="4">
-        <f t="shared" si="1"/>
+        <f t="shared" si="6"/>
         <v>190.7</v>
       </c>
       <c r="K44" s="4">
-        <f t="shared" si="1"/>
+        <f t="shared" si="6"/>
         <v>128.19999999999999</v>
       </c>
       <c r="L44" s="4">
-        <f t="shared" si="1"/>
+        <f t="shared" si="6"/>
         <v>227.3</v>
       </c>
       <c r="M44" s="4">
-        <f t="shared" si="1"/>
+        <f t="shared" si="6"/>
         <v>26.2</v>
       </c>
       <c r="N44" s="4">
-        <f t="shared" si="1"/>
+        <f t="shared" si="6"/>
         <v>225.8</v>
       </c>
       <c r="O44" s="4">
-        <f t="shared" si="1"/>
+        <f t="shared" si="6"/>
         <v>197.5</v>
       </c>
     </row>
     <row r="45" spans="1:18">
       <c r="A45" t="str">
-        <f t="shared" ref="A45:O48" si="2">A11</f>
+        <f t="shared" ref="A45:O48" si="7">A11</f>
         <v>push/pop</v>
       </c>
       <c r="B45" s="4">
-        <f t="shared" si="2"/>
+        <f t="shared" si="7"/>
         <v>71.2</v>
       </c>
       <c r="C45" s="4">
-        <f t="shared" si="2"/>
+        <f t="shared" si="7"/>
         <v>80.5</v>
       </c>
       <c r="D45" s="4">
-        <f t="shared" si="2"/>
+        <f t="shared" si="7"/>
         <v>60.3</v>
       </c>
       <c r="E45" s="4">
-        <f t="shared" si="2"/>
+        <f t="shared" si="7"/>
         <v>103.7</v>
       </c>
       <c r="F45" s="4">
-        <f t="shared" si="2"/>
+        <f t="shared" si="7"/>
         <v>133.30000000000001</v>
       </c>
       <c r="G45" s="4">
-        <f t="shared" si="2"/>
+        <f t="shared" si="7"/>
         <v>165.3</v>
       </c>
       <c r="H45" s="4">
-        <f t="shared" si="2"/>
+        <f t="shared" si="7"/>
         <v>52.6</v>
       </c>
       <c r="I45" s="4">
-        <f t="shared" si="2"/>
+        <f t="shared" si="7"/>
         <v>86.3</v>
       </c>
       <c r="J45" s="4">
-        <f t="shared" si="2"/>
+        <f t="shared" si="7"/>
         <v>63.6</v>
       </c>
       <c r="K45" s="4">
-        <f t="shared" si="2"/>
+        <f t="shared" si="7"/>
         <v>55.2</v>
       </c>
       <c r="L45" s="4">
-        <f t="shared" si="2"/>
+        <f t="shared" si="7"/>
         <v>72.8</v>
       </c>
       <c r="M45" s="4">
-        <f t="shared" si="2"/>
+        <f t="shared" si="7"/>
         <v>31.7</v>
       </c>
       <c r="N45" s="4">
-        <f t="shared" si="2"/>
+        <f t="shared" si="7"/>
         <v>83.3</v>
       </c>
       <c r="O45" s="4">
-        <f t="shared" si="2"/>
+        <f t="shared" si="7"/>
         <v>81.5</v>
       </c>
     </row>
     <row r="46" spans="1:18">
       <c r="A46" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="7"/>
         <v>load/store</v>
       </c>
       <c r="B46" s="4">
-        <f t="shared" si="2"/>
+        <f t="shared" si="7"/>
         <v>88.1</v>
       </c>
       <c r="C46" s="4">
-        <f t="shared" si="2"/>
+        <f t="shared" si="7"/>
         <v>73.8</v>
       </c>
       <c r="D46" s="4">
-        <f t="shared" si="2"/>
+        <f t="shared" si="7"/>
         <v>74</v>
       </c>
       <c r="E46" s="4">
-        <f t="shared" si="2"/>
+        <f t="shared" si="7"/>
         <v>28.4</v>
       </c>
       <c r="F46" s="4">
-        <f t="shared" si="2"/>
+        <f t="shared" si="7"/>
         <v>56.7</v>
       </c>
       <c r="G46" s="4">
-        <f t="shared" si="2"/>
+        <f t="shared" si="7"/>
         <v>67.900000000000006</v>
       </c>
       <c r="H46" s="4">
-        <f t="shared" si="2"/>
+        <f t="shared" si="7"/>
         <v>19.7</v>
       </c>
       <c r="I46" s="4">
-        <f t="shared" si="2"/>
+        <f t="shared" si="7"/>
         <v>101.1</v>
       </c>
       <c r="J46" s="4">
-        <f t="shared" si="2"/>
+        <f t="shared" si="7"/>
         <v>72.900000000000006</v>
       </c>
       <c r="K46" s="4">
-        <f t="shared" si="2"/>
+        <f t="shared" si="7"/>
         <v>45.8</v>
       </c>
       <c r="L46" s="4">
-        <f t="shared" si="2"/>
+        <f t="shared" si="7"/>
         <v>68.2</v>
       </c>
       <c r="M46" s="4">
-        <f t="shared" si="2"/>
+        <f t="shared" si="7"/>
         <v>22.6</v>
       </c>
       <c r="N46" s="4">
-        <f t="shared" si="2"/>
+        <f t="shared" si="7"/>
         <v>60.1</v>
       </c>
       <c r="O46" s="4">
-        <f t="shared" si="2"/>
+        <f t="shared" si="7"/>
         <v>59.9</v>
       </c>
     </row>
     <row r="47" spans="1:18">
       <c r="A47" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="7"/>
         <v>mov(w)</v>
       </c>
       <c r="B47" s="4">
-        <f t="shared" si="2"/>
+        <f t="shared" si="7"/>
         <v>10.199999999999999</v>
       </c>
       <c r="C47" s="4">
-        <f t="shared" si="2"/>
+        <f t="shared" si="7"/>
         <v>9.4</v>
       </c>
       <c r="D47" s="4">
-        <f t="shared" si="2"/>
+        <f t="shared" si="7"/>
         <v>4.0999999999999996</v>
       </c>
       <c r="E47" s="4">
-        <f t="shared" si="2"/>
+        <f t="shared" si="7"/>
         <v>2.6</v>
       </c>
       <c r="F47" s="4">
-        <f t="shared" si="2"/>
+        <f t="shared" si="7"/>
         <v>-1</v>
       </c>
       <c r="G47" s="4">
-        <f t="shared" si="2"/>
+        <f t="shared" si="7"/>
         <v>2.2000000000000002</v>
       </c>
       <c r="H47" s="4">
-        <f t="shared" si="2"/>
+        <f t="shared" si="7"/>
         <v>4.3</v>
       </c>
       <c r="I47" s="4">
-        <f t="shared" si="2"/>
+        <f t="shared" si="7"/>
         <v>4.7</v>
       </c>
       <c r="J47" s="4">
-        <f t="shared" si="2"/>
+        <f t="shared" si="7"/>
         <v>5.7</v>
       </c>
       <c r="K47" s="4">
-        <f t="shared" si="2"/>
+        <f t="shared" si="7"/>
         <v>-3.4</v>
       </c>
       <c r="L47" s="4">
-        <f t="shared" si="2"/>
+        <f t="shared" si="7"/>
         <v>19.600000000000001</v>
       </c>
       <c r="M47" s="4">
-        <f t="shared" si="2"/>
+        <f t="shared" si="7"/>
         <v>-14.3</v>
       </c>
       <c r="N47" s="4">
-        <f t="shared" si="2"/>
+        <f t="shared" si="7"/>
         <v>16.2</v>
       </c>
       <c r="O47" s="4">
-        <f t="shared" si="2"/>
+        <f t="shared" si="7"/>
         <v>4.5999999999999996</v>
       </c>
     </row>
     <row r="48" spans="1:18">
       <c r="A48" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="7"/>
         <v>other</v>
       </c>
       <c r="B48" s="4">
-        <f t="shared" si="2"/>
+        <f t="shared" si="7"/>
         <v>84.7</v>
       </c>
       <c r="C48" s="4">
-        <f t="shared" si="2"/>
+        <f t="shared" si="7"/>
         <v>75.8</v>
       </c>
       <c r="D48" s="4">
-        <f t="shared" si="2"/>
+        <f t="shared" si="7"/>
         <v>43.8</v>
       </c>
       <c r="E48" s="4">
-        <f t="shared" si="2"/>
+        <f t="shared" si="7"/>
         <v>28.2</v>
       </c>
       <c r="F48" s="4">
-        <f t="shared" si="2"/>
+        <f t="shared" si="7"/>
         <v>22.9</v>
       </c>
       <c r="G48" s="4">
-        <f t="shared" si="2"/>
+        <f t="shared" si="7"/>
         <v>114.1</v>
       </c>
       <c r="H48" s="4">
-        <f t="shared" si="2"/>
+        <f t="shared" si="7"/>
         <v>22.8</v>
       </c>
       <c r="I48" s="4">
-        <f t="shared" si="2"/>
+        <f t="shared" si="7"/>
         <v>76.8</v>
       </c>
       <c r="J48" s="4">
-        <f t="shared" si="2"/>
+        <f t="shared" si="7"/>
         <v>48.6</v>
       </c>
       <c r="K48" s="4">
-        <f t="shared" si="2"/>
+        <f t="shared" si="7"/>
         <v>30.5</v>
       </c>
       <c r="L48" s="4">
-        <f t="shared" si="2"/>
+        <f t="shared" si="7"/>
         <v>66.7</v>
       </c>
       <c r="M48" s="4">
-        <f t="shared" si="2"/>
+        <f t="shared" si="7"/>
         <v>-13.8</v>
       </c>
       <c r="N48" s="4">
-        <f t="shared" si="2"/>
+        <f t="shared" si="7"/>
         <v>66.2</v>
       </c>
       <c r="O48" s="4">
-        <f t="shared" si="2"/>
+        <f t="shared" si="7"/>
         <v>51.3</v>
       </c>
       <c r="Q48" s="10" t="s">
@@ -3583,59 +3583,59 @@
         <v>112</v>
       </c>
       <c r="B50" s="4">
-        <f>B18-B17</f>
+        <f t="shared" ref="B50:O50" si="8">B18-B17</f>
         <v>-67.799999999999983</v>
       </c>
       <c r="C50" s="4">
-        <f>C18-C17</f>
+        <f t="shared" si="8"/>
         <v>-53</v>
       </c>
       <c r="D50" s="4">
-        <f>D18-D17</f>
+        <f t="shared" si="8"/>
         <v>-45.199999999999989</v>
       </c>
       <c r="E50" s="4">
-        <f>E18-E17</f>
+        <f t="shared" si="8"/>
         <v>-38.299999999999997</v>
       </c>
       <c r="F50" s="4">
-        <f>F18-F17</f>
+        <f t="shared" si="8"/>
         <v>-49.400000000000006</v>
       </c>
       <c r="G50" s="4">
-        <f>G18-G17</f>
+        <f t="shared" si="8"/>
         <v>-62.5</v>
       </c>
       <c r="H50" s="4">
-        <f>H18-H17</f>
+        <f t="shared" si="8"/>
         <v>-32.200000000000003</v>
       </c>
       <c r="I50" s="4">
-        <f>I18-I17</f>
+        <f t="shared" si="8"/>
         <v>-77.799999999999983</v>
       </c>
       <c r="J50" s="4">
-        <f>J18-J17</f>
+        <f t="shared" si="8"/>
         <v>-33.899999999999977</v>
       </c>
       <c r="K50" s="4">
-        <f>K18-K17</f>
+        <f t="shared" si="8"/>
         <v>-24.699999999999989</v>
       </c>
       <c r="L50" s="4">
-        <f>L18-L17</f>
+        <f t="shared" si="8"/>
         <v>-27.400000000000006</v>
       </c>
       <c r="M50" s="4">
-        <f>M18-M17</f>
+        <f t="shared" si="8"/>
         <v>-13.6</v>
       </c>
       <c r="N50" s="4">
-        <f>N18-N17</f>
+        <f t="shared" si="8"/>
         <v>-49.800000000000011</v>
       </c>
       <c r="O50" s="4">
-        <f>O18-O17</f>
+        <f t="shared" si="8"/>
         <v>-44.300000000000011</v>
       </c>
     </row>
@@ -3644,59 +3644,59 @@
         <v>23</v>
       </c>
       <c r="B51" s="4">
-        <f>B19-B18</f>
+        <f t="shared" ref="B51:O51" si="9">B19-B18</f>
         <v>-25.400000000000006</v>
       </c>
       <c r="C51" s="4">
-        <f>C19-C18</f>
+        <f t="shared" si="9"/>
         <v>-26.199999999999989</v>
       </c>
       <c r="D51" s="4">
-        <f>D19-D18</f>
+        <f t="shared" si="9"/>
         <v>-24.700000000000003</v>
       </c>
       <c r="E51" s="4">
-        <f>E19-E18</f>
+        <f t="shared" si="9"/>
         <v>-59.400000000000006</v>
       </c>
       <c r="F51" s="4">
-        <f>F19-F18</f>
+        <f t="shared" si="9"/>
         <v>-85.4</v>
       </c>
       <c r="G51" s="4">
-        <f>G19-G18</f>
+        <f t="shared" si="9"/>
         <v>-111.19999999999999</v>
       </c>
       <c r="H51" s="4">
-        <f>H19-H18</f>
+        <f t="shared" si="9"/>
         <v>-20.900000000000006</v>
       </c>
       <c r="I51" s="4">
-        <f>I19-I18</f>
+        <f t="shared" si="9"/>
         <v>-30.599999999999994</v>
       </c>
       <c r="J51" s="4">
-        <f>J19-J18</f>
+        <f t="shared" si="9"/>
         <v>-39.700000000000017</v>
       </c>
       <c r="K51" s="4">
-        <f>K19-K18</f>
+        <f t="shared" si="9"/>
         <v>-27.599999999999994</v>
       </c>
       <c r="L51" s="4">
-        <f>L19-L18</f>
+        <f t="shared" si="9"/>
         <v>-26.700000000000017</v>
       </c>
       <c r="M51" s="4">
-        <f>M19-M18</f>
+        <f t="shared" si="9"/>
         <v>-12.6</v>
       </c>
       <c r="N51" s="4">
-        <f>N19-N18</f>
+        <f t="shared" si="9"/>
         <v>-38.300000000000011</v>
       </c>
       <c r="O51" s="4">
-        <f>O19-O18</f>
+        <f t="shared" si="9"/>
         <v>-40.699999999999989</v>
       </c>
     </row>
@@ -3705,59 +3705,59 @@
         <v>24</v>
       </c>
       <c r="B52" s="4">
-        <f>B20-B19</f>
+        <f t="shared" ref="B52:O52" si="10">B20-B19</f>
         <v>-16.900000000000006</v>
       </c>
       <c r="C52" s="4">
-        <f>C20-C19</f>
+        <f t="shared" si="10"/>
         <v>-29.5</v>
       </c>
       <c r="D52" s="4">
-        <f>D20-D19</f>
+        <f t="shared" si="10"/>
         <v>-6.7999999999999972</v>
       </c>
       <c r="E52" s="4">
-        <f>E20-E19</f>
+        <f t="shared" si="10"/>
         <v>-6.1999999999999957</v>
       </c>
       <c r="F52" s="4">
-        <f>F20-F19</f>
+        <f t="shared" si="10"/>
         <v>-18.699999999999996</v>
       </c>
       <c r="G52" s="4">
-        <f>G20-G19</f>
+        <f t="shared" si="10"/>
         <v>-18.700000000000017</v>
       </c>
       <c r="H52" s="4">
-        <f>H20-H19</f>
+        <f t="shared" si="10"/>
         <v>-13.5</v>
       </c>
       <c r="I52" s="4">
-        <f>I20-I19</f>
+        <f t="shared" si="10"/>
         <v>-5.1999999999999886</v>
       </c>
       <c r="J52" s="4">
-        <f>J20-J19</f>
+        <f t="shared" si="10"/>
         <v>-18.5</v>
       </c>
       <c r="K52" s="4">
-        <f>K20-K19</f>
+        <f t="shared" si="10"/>
         <v>-9.9000000000000057</v>
       </c>
       <c r="L52" s="4">
-        <f>L20-L19</f>
+        <f t="shared" si="10"/>
         <v>-26.699999999999989</v>
       </c>
       <c r="M52" s="4">
-        <f>M20-M19</f>
+        <f t="shared" si="10"/>
         <v>-8.1</v>
       </c>
       <c r="N52" s="4">
-        <f>N20-N19</f>
+        <f t="shared" si="10"/>
         <v>-20.699999999999989</v>
       </c>
       <c r="O52" s="4">
-        <f>O20-O19</f>
+        <f t="shared" si="10"/>
         <v>-15.299999999999997</v>
       </c>
     </row>
@@ -3766,59 +3766,59 @@
         <v>25</v>
       </c>
       <c r="B53" s="4">
-        <f>B21-B20</f>
+        <f t="shared" ref="B53:O53" si="11">B21-B20</f>
         <v>1.7000000000000171</v>
       </c>
       <c r="C53" s="4">
-        <f>C21-C20</f>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
       <c r="D53" s="4">
-        <f>D21-D20</f>
+        <f t="shared" si="11"/>
         <v>21.900000000000006</v>
       </c>
       <c r="E53" s="4">
-        <f>E21-E20</f>
+        <f t="shared" si="11"/>
         <v>5.8999999999999986</v>
       </c>
       <c r="F53" s="4">
-        <f>F21-F20</f>
+        <f t="shared" si="11"/>
         <v>-1.1999999999999957</v>
       </c>
       <c r="G53" s="4">
-        <f>G21-G20</f>
+        <f t="shared" si="11"/>
         <v>-2.5999999999999943</v>
       </c>
       <c r="H53" s="4">
-        <f>H21-H20</f>
+        <f t="shared" si="11"/>
         <v>-4.1999999999999957</v>
       </c>
       <c r="I53" s="4">
-        <f>I21-I20</f>
+        <f t="shared" si="11"/>
         <v>-16.400000000000006</v>
       </c>
       <c r="J53" s="4">
-        <f>J21-J20</f>
+        <f t="shared" si="11"/>
         <v>2.5</v>
       </c>
       <c r="K53" s="4">
-        <f>K21-K20</f>
+        <f t="shared" si="11"/>
         <v>-1.5</v>
       </c>
       <c r="L53" s="4">
-        <f>L21-L20</f>
+        <f t="shared" si="11"/>
         <v>-8.6999999999999886</v>
       </c>
       <c r="M53" s="4">
-        <f>M21-M20</f>
+        <f t="shared" si="11"/>
         <v>-1.3000000000000007</v>
       </c>
       <c r="N53" s="4">
-        <f>N21-N20</f>
+        <f t="shared" si="11"/>
         <v>-11.400000000000006</v>
       </c>
       <c r="O53" s="4">
-        <f>O21-O20</f>
+        <f t="shared" si="11"/>
         <v>-1.2000000000000028</v>
       </c>
     </row>
@@ -3827,59 +3827,59 @@
         <v>26</v>
       </c>
       <c r="B54" s="4">
-        <f>B22-B21</f>
+        <f t="shared" ref="B54:O54" si="12">B22-B21</f>
         <v>0</v>
       </c>
       <c r="C54" s="4">
-        <f>C22-C21</f>
+        <f t="shared" si="12"/>
         <v>-6.1000000000000085</v>
       </c>
       <c r="D54" s="4">
-        <f>D22-D21</f>
+        <f t="shared" si="12"/>
         <v>-6.9000000000000057</v>
       </c>
       <c r="E54" s="4">
-        <f>E22-E21</f>
+        <f t="shared" si="12"/>
         <v>1.7000000000000028</v>
       </c>
       <c r="F54" s="4">
-        <f>F22-F21</f>
+        <f t="shared" si="12"/>
         <v>2.7999999999999972</v>
       </c>
       <c r="G54" s="4">
-        <f>G22-G21</f>
+        <f t="shared" si="12"/>
         <v>-16</v>
       </c>
       <c r="H54" s="4">
-        <f>H22-H21</f>
+        <f t="shared" si="12"/>
         <v>-4.6000000000000014</v>
       </c>
       <c r="I54" s="4">
-        <f>I22-I21</f>
+        <f t="shared" si="12"/>
         <v>-2.5999999999999943</v>
       </c>
       <c r="J54" s="4">
-        <f>J22-J21</f>
+        <f t="shared" si="12"/>
         <v>-1.7999999999999972</v>
       </c>
       <c r="K54" s="4">
-        <f>K22-K21</f>
+        <f t="shared" si="12"/>
         <v>-1.5</v>
       </c>
       <c r="L54" s="4">
-        <f>L22-L21</f>
+        <f t="shared" si="12"/>
         <v>0</v>
       </c>
       <c r="M54" s="4">
-        <f>M22-M21</f>
+        <f t="shared" si="12"/>
         <v>-1.6999999999999993</v>
       </c>
       <c r="N54" s="4">
-        <f>N22-N21</f>
+        <f t="shared" si="12"/>
         <v>-9.9999999999994316E-2</v>
       </c>
       <c r="O54" s="4">
-        <f>O22-O21</f>
+        <f t="shared" si="12"/>
         <v>-2.7999999999999972</v>
       </c>
     </row>
@@ -3888,59 +3888,59 @@
         <v>27</v>
       </c>
       <c r="B55" s="4">
-        <f>B23-B22</f>
+        <f t="shared" ref="B55:O55" si="13">B23-B22</f>
         <v>-27.200000000000017</v>
       </c>
       <c r="C55" s="4">
-        <f>C23-C22</f>
+        <f t="shared" si="13"/>
         <v>-22.799999999999997</v>
       </c>
       <c r="D55" s="4">
-        <f>D23-D22</f>
+        <f t="shared" si="13"/>
         <v>-8.2000000000000028</v>
       </c>
       <c r="E55" s="4">
-        <f>E23-E22</f>
+        <f t="shared" si="13"/>
         <v>-11.600000000000001</v>
       </c>
       <c r="F55" s="4">
-        <f>F23-F22</f>
+        <f t="shared" si="13"/>
         <v>-5.1000000000000014</v>
       </c>
       <c r="G55" s="4">
-        <f>G23-G22</f>
+        <f t="shared" si="13"/>
         <v>-16.700000000000003</v>
       </c>
       <c r="H55" s="4">
-        <f>H23-H22</f>
+        <f t="shared" si="13"/>
         <v>-11.6</v>
       </c>
       <c r="I55" s="4">
-        <f>I23-I22</f>
+        <f t="shared" si="13"/>
         <v>-25.800000000000011</v>
       </c>
       <c r="J55" s="4">
-        <f>J23-J22</f>
+        <f t="shared" si="13"/>
         <v>-10.700000000000003</v>
       </c>
       <c r="K55" s="4">
-        <f>K23-K22</f>
+        <f t="shared" si="13"/>
         <v>-7.3999999999999986</v>
       </c>
       <c r="L55" s="4">
-        <f>L23-L22</f>
+        <f t="shared" si="13"/>
         <v>-16.900000000000006</v>
       </c>
       <c r="M55" s="4">
-        <f>M23-M22</f>
+        <f t="shared" si="13"/>
         <v>-2.2000000000000011</v>
       </c>
       <c r="N55" s="4">
-        <f>N23-N22</f>
+        <f t="shared" si="13"/>
         <v>-10.700000000000003</v>
       </c>
       <c r="O55" s="4">
-        <f>O23-O22</f>
+        <f t="shared" si="13"/>
         <v>-13.600000000000009</v>
       </c>
     </row>
@@ -3949,59 +3949,59 @@
         <v>28</v>
       </c>
       <c r="B56" s="4">
-        <f>B24-B23</f>
+        <f t="shared" ref="B56:O56" si="14">B24-B23</f>
         <v>0</v>
       </c>
       <c r="C56" s="4">
-        <f>C24-C23</f>
+        <f t="shared" si="14"/>
         <v>0</v>
       </c>
       <c r="D56" s="4">
-        <f>D24-D23</f>
+        <f t="shared" si="14"/>
         <v>0</v>
       </c>
       <c r="E56" s="4">
-        <f>E24-E23</f>
+        <f t="shared" si="14"/>
         <v>0</v>
       </c>
       <c r="F56" s="4">
-        <f>F24-F23</f>
+        <f t="shared" si="14"/>
         <v>0</v>
       </c>
       <c r="G56" s="4">
-        <f>G24-G23</f>
+        <f t="shared" si="14"/>
         <v>0</v>
       </c>
       <c r="H56" s="4">
-        <f>H24-H23</f>
+        <f t="shared" si="14"/>
         <v>-9.9</v>
       </c>
       <c r="I56" s="4">
-        <f>I24-I23</f>
+        <f t="shared" si="14"/>
         <v>0</v>
       </c>
       <c r="J56" s="4">
-        <f>J24-J23</f>
+        <f t="shared" si="14"/>
         <v>0</v>
       </c>
       <c r="K56" s="4">
-        <f>K24-K23</f>
+        <f t="shared" si="14"/>
         <v>-3.3999999999999986</v>
       </c>
       <c r="L56" s="4">
-        <f>L24-L23</f>
+        <f t="shared" si="14"/>
         <v>0</v>
       </c>
       <c r="M56" s="4">
-        <f>M24-M23</f>
+        <f t="shared" si="14"/>
         <v>0</v>
       </c>
       <c r="N56" s="4">
-        <f>N24-N23</f>
+        <f t="shared" si="14"/>
         <v>0</v>
       </c>
       <c r="O56" s="4">
-        <f>O24-O23</f>
+        <f t="shared" si="14"/>
         <v>-1.0999999999999943</v>
       </c>
     </row>
@@ -4010,59 +4010,59 @@
         <v>29</v>
       </c>
       <c r="B57" s="4">
-        <f>B25-B24</f>
+        <f t="shared" ref="B57:O57" si="15">B25-B24</f>
         <v>0</v>
       </c>
       <c r="C57" s="4">
-        <f>C25-C24</f>
+        <f t="shared" si="15"/>
         <v>-2</v>
       </c>
       <c r="D57" s="4">
-        <f>D25-D24</f>
+        <f t="shared" si="15"/>
         <v>0</v>
       </c>
       <c r="E57" s="4">
-        <f>E25-E24</f>
+        <f t="shared" si="15"/>
         <v>0</v>
       </c>
       <c r="F57" s="4">
-        <f>F25-F24</f>
+        <f t="shared" si="15"/>
         <v>0</v>
       </c>
       <c r="G57" s="4">
-        <f>G25-G24</f>
+        <f t="shared" si="15"/>
         <v>0</v>
       </c>
       <c r="H57" s="4">
-        <f>H25-H24</f>
+        <f t="shared" si="15"/>
         <v>0</v>
       </c>
       <c r="I57" s="4">
-        <f>I25-I24</f>
+        <f t="shared" si="15"/>
         <v>0</v>
       </c>
       <c r="J57" s="4">
-        <f>J25-J24</f>
+        <f t="shared" si="15"/>
         <v>0</v>
       </c>
       <c r="K57" s="4">
-        <f>K25-K24</f>
+        <f t="shared" si="15"/>
         <v>-5.5</v>
       </c>
       <c r="L57" s="4">
-        <f>L25-L24</f>
+        <f t="shared" si="15"/>
         <v>-3.8000000000000114</v>
       </c>
       <c r="M57" s="4">
-        <f>M25-M24</f>
+        <f t="shared" si="15"/>
         <v>-3.8999999999999986</v>
       </c>
       <c r="N57" s="4">
-        <f>N25-N24</f>
+        <f t="shared" si="15"/>
         <v>0.60000000000000853</v>
       </c>
       <c r="O57" s="4">
-        <f>O25-O24</f>
+        <f t="shared" si="15"/>
         <v>-1.0999999999999943</v>
       </c>
     </row>
@@ -4090,59 +4090,59 @@
         <v>14</v>
       </c>
       <c r="B59" s="4">
-        <f>B27</f>
+        <f t="shared" ref="B59:O59" si="16">B27</f>
         <v>118.6</v>
       </c>
       <c r="C59" s="4">
-        <f>C27</f>
+        <f t="shared" si="16"/>
         <v>100</v>
       </c>
       <c r="D59" s="4">
-        <f>D27</f>
+        <f t="shared" si="16"/>
         <v>112.3</v>
       </c>
       <c r="E59" s="4">
-        <f>E27</f>
+        <f t="shared" si="16"/>
         <v>55.1</v>
       </c>
       <c r="F59" s="4">
-        <f>F27</f>
+        <f t="shared" si="16"/>
         <v>54.9</v>
       </c>
       <c r="G59" s="4">
-        <f>G27</f>
+        <f t="shared" si="16"/>
         <v>121.8</v>
       </c>
       <c r="H59" s="4">
-        <f>H27</f>
+        <f t="shared" si="16"/>
         <v>2.5</v>
       </c>
       <c r="I59" s="4">
-        <f>I27</f>
+        <f t="shared" si="16"/>
         <v>110.5</v>
       </c>
       <c r="J59" s="4">
-        <f>J27</f>
+        <f t="shared" si="16"/>
         <v>88.6</v>
       </c>
       <c r="K59" s="4">
-        <f>K27</f>
+        <f t="shared" si="16"/>
         <v>46.7</v>
       </c>
       <c r="L59" s="4">
-        <f>L27</f>
+        <f t="shared" si="16"/>
         <v>117.1</v>
       </c>
       <c r="M59" s="4">
-        <f>M27</f>
+        <f t="shared" si="16"/>
         <v>-17.2</v>
       </c>
       <c r="N59" s="4">
-        <f>N27</f>
+        <f t="shared" si="16"/>
         <v>95.4</v>
       </c>
       <c r="O59" s="4">
-        <f>O27</f>
+        <f t="shared" si="16"/>
         <v>77.400000000000006</v>
       </c>
     </row>
@@ -4151,59 +4151,59 @@
         <v>15</v>
       </c>
       <c r="B60" s="4">
-        <f>B28</f>
+        <f t="shared" ref="B60:O60" si="17">B28</f>
         <v>23.7</v>
       </c>
       <c r="C60" s="4">
-        <f>C28</f>
+        <f t="shared" si="17"/>
         <v>16.100000000000001</v>
       </c>
       <c r="D60" s="4">
-        <f>D28</f>
+        <f t="shared" si="17"/>
         <v>27.4</v>
       </c>
       <c r="E60" s="4">
-        <f>E28</f>
+        <f t="shared" si="17"/>
         <v>13.3</v>
       </c>
       <c r="F60" s="4">
-        <f>F28</f>
+        <f t="shared" si="17"/>
         <v>0</v>
       </c>
       <c r="G60" s="4">
-        <f>G28</f>
+        <f t="shared" si="17"/>
         <v>6.2</v>
       </c>
       <c r="H60" s="4">
-        <f>H28</f>
+        <f t="shared" si="17"/>
         <v>1.9</v>
       </c>
       <c r="I60" s="4">
-        <f>I28</f>
+        <f t="shared" si="17"/>
         <v>-2.1</v>
       </c>
       <c r="J60" s="4">
-        <f>J28</f>
+        <f t="shared" si="17"/>
         <v>-5</v>
       </c>
       <c r="K60" s="4">
-        <f>K28</f>
+        <f t="shared" si="17"/>
         <v>1.7</v>
       </c>
       <c r="L60" s="4">
-        <f>L28</f>
+        <f t="shared" si="17"/>
         <v>16.3</v>
       </c>
       <c r="M60" s="4">
-        <f>M28</f>
+        <f t="shared" si="17"/>
         <v>3.9</v>
       </c>
       <c r="N60" s="4">
-        <f>N28</f>
+        <f t="shared" si="17"/>
         <v>-3.1</v>
       </c>
       <c r="O60" s="4">
-        <f>O28</f>
+        <f t="shared" si="17"/>
         <v>7.7</v>
       </c>
     </row>
@@ -4212,59 +4212,59 @@
         <v>16</v>
       </c>
       <c r="B61" s="4">
-        <f>B29</f>
+        <f t="shared" ref="B61:O61" si="18">B29</f>
         <v>33.9</v>
       </c>
       <c r="C61" s="4">
-        <f>C29</f>
+        <f t="shared" si="18"/>
         <v>41.6</v>
       </c>
       <c r="D61" s="4">
-        <f>D29</f>
+        <f t="shared" si="18"/>
         <v>49.3</v>
       </c>
       <c r="E61" s="4">
-        <f>E29</f>
+        <f t="shared" si="18"/>
         <v>14.8</v>
       </c>
       <c r="F61" s="4">
-        <f>F29</f>
+        <f t="shared" si="18"/>
         <v>37.200000000000003</v>
       </c>
       <c r="G61" s="4">
-        <f>G29</f>
+        <f t="shared" si="18"/>
         <v>25.3</v>
       </c>
       <c r="H61" s="4">
-        <f>H29</f>
+        <f t="shared" si="18"/>
         <v>-2.6</v>
       </c>
       <c r="I61" s="4">
-        <f>I29</f>
+        <f t="shared" si="18"/>
         <v>57.9</v>
       </c>
       <c r="J61" s="4">
-        <f>J29</f>
+        <f t="shared" si="18"/>
         <v>45</v>
       </c>
       <c r="K61" s="4">
-        <f>K29</f>
+        <f t="shared" si="18"/>
         <v>30.1</v>
       </c>
       <c r="L61" s="4">
-        <f>L29</f>
+        <f t="shared" si="18"/>
         <v>40.9</v>
       </c>
       <c r="M61" s="4">
-        <f>M29</f>
+        <f t="shared" si="18"/>
         <v>8</v>
       </c>
       <c r="N61" s="4">
-        <f>N29</f>
+        <f t="shared" si="18"/>
         <v>37.6</v>
       </c>
       <c r="O61" s="4">
-        <f>O29</f>
+        <f t="shared" si="18"/>
         <v>32.200000000000003</v>
       </c>
     </row>
@@ -4273,59 +4273,59 @@
         <v>17</v>
       </c>
       <c r="B62" s="4">
-        <f>B30</f>
+        <f t="shared" ref="B62:O62" si="19">B30</f>
         <v>1.7</v>
       </c>
       <c r="C62" s="4">
-        <f>C30</f>
+        <f t="shared" si="19"/>
         <v>6.7</v>
       </c>
       <c r="D62" s="4">
-        <f>D30</f>
+        <f t="shared" si="19"/>
         <v>6.8</v>
       </c>
       <c r="E62" s="4">
-        <f>E30</f>
+        <f t="shared" si="19"/>
         <v>2.5</v>
       </c>
       <c r="F62" s="4">
-        <f>F30</f>
+        <f t="shared" si="19"/>
         <v>-2.4</v>
       </c>
       <c r="G62" s="4">
-        <f>G30</f>
+        <f t="shared" si="19"/>
         <v>11.9</v>
       </c>
       <c r="H62" s="4">
-        <f>H30</f>
+        <f t="shared" si="19"/>
         <v>-0.8</v>
       </c>
       <c r="I62" s="4">
-        <f>I30</f>
+        <f t="shared" si="19"/>
         <v>1.1000000000000001</v>
       </c>
       <c r="J62" s="4">
-        <f>J30</f>
+        <f t="shared" si="19"/>
         <v>7.1</v>
       </c>
       <c r="K62" s="4">
-        <f>K30</f>
+        <f t="shared" si="19"/>
         <v>-0.2</v>
       </c>
       <c r="L62" s="4">
-        <f>L30</f>
+        <f t="shared" si="19"/>
         <v>15.4</v>
       </c>
       <c r="M62" s="4">
-        <f>M30</f>
+        <f t="shared" si="19"/>
         <v>-10.7</v>
       </c>
       <c r="N62" s="4">
-        <f>N30</f>
+        <f t="shared" si="19"/>
         <v>13.3</v>
       </c>
       <c r="O62" s="4">
-        <f>O30</f>
+        <f t="shared" si="19"/>
         <v>4</v>
       </c>
     </row>
@@ -4334,59 +4334,59 @@
         <v>19</v>
       </c>
       <c r="B63" s="4">
-        <f>B31</f>
+        <f t="shared" ref="B63:O63" si="20">B31</f>
         <v>59.3</v>
       </c>
       <c r="C63" s="4">
-        <f>C31</f>
+        <f t="shared" si="20"/>
         <v>35.6</v>
       </c>
       <c r="D63" s="4">
-        <f>D31</f>
+        <f t="shared" si="20"/>
         <v>28.8</v>
       </c>
       <c r="E63" s="4">
-        <f>E31</f>
+        <f t="shared" si="20"/>
         <v>24.4</v>
       </c>
       <c r="F63" s="4">
-        <f>F31</f>
+        <f t="shared" si="20"/>
         <v>20.100000000000001</v>
       </c>
       <c r="G63" s="4">
-        <f>G31</f>
+        <f t="shared" si="20"/>
         <v>78.5</v>
       </c>
       <c r="H63" s="4">
-        <f>H31</f>
+        <f t="shared" si="20"/>
         <v>4</v>
       </c>
       <c r="I63" s="4">
-        <f>I31</f>
+        <f t="shared" si="20"/>
         <v>53.7</v>
       </c>
       <c r="J63" s="4">
-        <f>J31</f>
+        <f t="shared" si="20"/>
         <v>41.4</v>
       </c>
       <c r="K63" s="4">
-        <f>K31</f>
+        <f t="shared" si="20"/>
         <v>15.1</v>
       </c>
       <c r="L63" s="4">
-        <f>L31</f>
+        <f t="shared" si="20"/>
         <v>44.5</v>
       </c>
       <c r="M63" s="4">
-        <f>M31</f>
+        <f t="shared" si="20"/>
         <v>-18.399999999999999</v>
       </c>
       <c r="N63" s="4">
-        <f>N31</f>
+        <f t="shared" si="20"/>
         <v>47.6</v>
       </c>
       <c r="O63" s="4">
-        <f>O31</f>
+        <f t="shared" si="20"/>
         <v>33.4</v>
       </c>
     </row>
@@ -7858,7 +7858,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:U45"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
       <selection activeCell="I15" sqref="I15"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Added graph used in defence presentation and changed problem in a table
</commit_message>
<xml_diff>
--- a/data/maingraphs-code-size-table3a.xlsx
+++ b/data/maingraphs-code-size-table3a.xlsx
@@ -4,14 +4,13 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="28125"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16060" tabRatio="500" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="-20" windowWidth="33600" windowHeight="20540" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="main table" sheetId="1" r:id="rId1"/>
     <sheet name="graphs" sheetId="2" r:id="rId2"/>
     <sheet name="vm size break even table" sheetId="3" r:id="rId3"/>
     <sheet name="mem usage" sheetId="4" r:id="rId4"/>
-    <sheet name="Sheet1" sheetId="5" r:id="rId5"/>
   </sheets>
   <calcPr calcId="140000" concurrentCalc="0"/>
   <extLst>
@@ -23,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="355" uniqueCount="130">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="350" uniqueCount="130">
   <si>
     <t>BENCHMARK x</t>
   </si>
@@ -516,8 +515,10 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="339">
+  <cellStyleXfs count="341">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -872,7 +873,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
-  <cellStyles count="339">
+  <cellStyles count="341">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -1042,6 +1043,7 @@
     <cellStyle name="Followed Hyperlink" xfId="334" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="336" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="338" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="340" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -1211,6 +1213,7 @@
     <cellStyle name="Hyperlink" xfId="333" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="335" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="337" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="339" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1542,7 +1545,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:R66"/>
   <sheetViews>
-    <sheetView topLeftCell="A18" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B36" sqref="B36:O63"/>
     </sheetView>
   </sheetViews>
@@ -4421,8 +4424,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:T94"/>
   <sheetViews>
-    <sheetView topLeftCell="A62" workbookViewId="0">
-      <selection activeCell="N94" sqref="A84:N94"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A38" sqref="A38:XFD38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -7858,7 +7861,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:U45"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="I15" sqref="I15"/>
     </sheetView>
   </sheetViews>
@@ -9689,260 +9692,4 @@
     </ext>
   </extLst>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:O5"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:O5"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
-  <sheetData>
-    <row r="1" spans="1:15">
-      <c r="A1" t="s">
-        <v>14</v>
-      </c>
-      <c r="B1">
-        <v>254.2</v>
-      </c>
-      <c r="C1">
-        <v>239.6</v>
-      </c>
-      <c r="D1">
-        <v>182.2</v>
-      </c>
-      <c r="E1">
-        <v>163</v>
-      </c>
-      <c r="F1">
-        <v>211.9</v>
-      </c>
-      <c r="G1">
-        <v>349.5</v>
-      </c>
-      <c r="H1">
-        <v>99.4</v>
-      </c>
-      <c r="I1">
-        <v>268.89999999999998</v>
-      </c>
-      <c r="J1">
-        <v>190.7</v>
-      </c>
-      <c r="K1">
-        <v>128.19999999999999</v>
-      </c>
-      <c r="L1">
-        <v>227.3</v>
-      </c>
-      <c r="M1">
-        <v>26.2</v>
-      </c>
-      <c r="N1">
-        <v>225.8</v>
-      </c>
-      <c r="O1">
-        <v>197.5</v>
-      </c>
-    </row>
-    <row r="2" spans="1:15">
-      <c r="A2" t="s">
-        <v>15</v>
-      </c>
-      <c r="B2">
-        <v>71.2</v>
-      </c>
-      <c r="C2">
-        <v>80.5</v>
-      </c>
-      <c r="D2">
-        <v>60.3</v>
-      </c>
-      <c r="E2">
-        <v>103.7</v>
-      </c>
-      <c r="F2">
-        <v>133.30000000000001</v>
-      </c>
-      <c r="G2">
-        <v>165.3</v>
-      </c>
-      <c r="H2">
-        <v>52.6</v>
-      </c>
-      <c r="I2">
-        <v>86.3</v>
-      </c>
-      <c r="J2">
-        <v>63.6</v>
-      </c>
-      <c r="K2">
-        <v>55.2</v>
-      </c>
-      <c r="L2">
-        <v>72.8</v>
-      </c>
-      <c r="M2">
-        <v>31.7</v>
-      </c>
-      <c r="N2">
-        <v>83.3</v>
-      </c>
-      <c r="O2">
-        <v>81.5</v>
-      </c>
-    </row>
-    <row r="3" spans="1:15">
-      <c r="A3" t="s">
-        <v>16</v>
-      </c>
-      <c r="B3">
-        <v>88.1</v>
-      </c>
-      <c r="C3">
-        <v>73.8</v>
-      </c>
-      <c r="D3">
-        <v>74</v>
-      </c>
-      <c r="E3">
-        <v>28.4</v>
-      </c>
-      <c r="F3">
-        <v>56.7</v>
-      </c>
-      <c r="G3">
-        <v>67.900000000000006</v>
-      </c>
-      <c r="H3">
-        <v>19.7</v>
-      </c>
-      <c r="I3">
-        <v>101.1</v>
-      </c>
-      <c r="J3">
-        <v>72.900000000000006</v>
-      </c>
-      <c r="K3">
-        <v>45.8</v>
-      </c>
-      <c r="L3">
-        <v>68.2</v>
-      </c>
-      <c r="M3">
-        <v>22.6</v>
-      </c>
-      <c r="N3">
-        <v>60.1</v>
-      </c>
-      <c r="O3">
-        <v>59.9</v>
-      </c>
-    </row>
-    <row r="4" spans="1:15">
-      <c r="A4" t="s">
-        <v>17</v>
-      </c>
-      <c r="B4">
-        <v>10.199999999999999</v>
-      </c>
-      <c r="C4">
-        <v>9.4</v>
-      </c>
-      <c r="D4">
-        <v>4.0999999999999996</v>
-      </c>
-      <c r="E4">
-        <v>2.6</v>
-      </c>
-      <c r="F4">
-        <v>-1</v>
-      </c>
-      <c r="G4">
-        <v>2.2000000000000002</v>
-      </c>
-      <c r="H4">
-        <v>4.3</v>
-      </c>
-      <c r="I4">
-        <v>4.7</v>
-      </c>
-      <c r="J4">
-        <v>5.7</v>
-      </c>
-      <c r="K4">
-        <v>-3.4</v>
-      </c>
-      <c r="L4">
-        <v>19.600000000000001</v>
-      </c>
-      <c r="M4">
-        <v>-14.3</v>
-      </c>
-      <c r="N4">
-        <v>16.2</v>
-      </c>
-      <c r="O4">
-        <v>4.5999999999999996</v>
-      </c>
-    </row>
-    <row r="5" spans="1:15">
-      <c r="A5" t="s">
-        <v>19</v>
-      </c>
-      <c r="B5">
-        <v>84.7</v>
-      </c>
-      <c r="C5">
-        <v>75.8</v>
-      </c>
-      <c r="D5">
-        <v>43.8</v>
-      </c>
-      <c r="E5">
-        <v>28.2</v>
-      </c>
-      <c r="F5">
-        <v>22.9</v>
-      </c>
-      <c r="G5">
-        <v>114.1</v>
-      </c>
-      <c r="H5">
-        <v>22.8</v>
-      </c>
-      <c r="I5">
-        <v>76.8</v>
-      </c>
-      <c r="J5">
-        <v>48.6</v>
-      </c>
-      <c r="K5">
-        <v>30.5</v>
-      </c>
-      <c r="L5">
-        <v>66.7</v>
-      </c>
-      <c r="M5">
-        <v>-13.8</v>
-      </c>
-      <c r="N5">
-        <v>66.2</v>
-      </c>
-      <c r="O5">
-        <v>51.3</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
-</worksheet>
 </file>
</xml_diff>